<commit_message>
Improved handling of missing numbers
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yhata\OneDrive\デスクトップ\GIT\xlsx2json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316AB185-D197-467B-8EE7-865C80372F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F727E1C2-DEBA-44D3-8C80-5A0D973B3190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,12 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="json.customer_name">Sheet1!$G$4</definedName>
+    <definedName name="json.customer.address">Sheet1!$G$8</definedName>
+    <definedName name="json.customer.name">Sheet1!$G$7</definedName>
     <definedName name="json.parent.1">Sheet1!$G$2:$H$2</definedName>
     <definedName name="json.parent.2">Sheet1!$G$3:$H$3</definedName>
+    <definedName name="json.parent.3">Sheet1!$G$4:$H$4</definedName>
+    <definedName name="json.parent.4">Sheet1!$G$5:$H$5</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,33 +33,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>parent</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>child</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>customer_name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>A</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>D</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -64,6 +47,41 @@
     <rPh sb="0" eb="4">
       <t>ヤマダタロウ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>G2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>H2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>G3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>H3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>H5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>address</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>とうきょう</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -389,9 +407,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
   <cols>
@@ -426,15 +444,42 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" t="s">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
-        <v>7</v>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Wildcard matching of correct item names from JSON Schema
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yhata\OneDrive\デスクトップ\GIT\xlsx2json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F727E1C2-DEBA-44D3-8C80-5A0D973B3190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBAA1AC-46AA-4F90-B408-362C89F6449E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,8 @@
     <definedName name="json.parent.2">Sheet1!$G$3:$H$3</definedName>
     <definedName name="json.parent.3">Sheet1!$G$4:$H$4</definedName>
     <definedName name="json.parent.4">Sheet1!$G$5:$H$5</definedName>
+    <definedName name="json.日本語_._記_号__">Sheet1!$G$11</definedName>
+    <definedName name="json.日本語_.記号_">Sheet1!$G$10</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>parent</t>
     <phoneticPr fontId="1"/>
@@ -82,6 +84,35 @@
   </si>
   <si>
     <t>とうきょう</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>エラーにならない～！</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>記号！</t>
+    <rPh sb="0" eb="2">
+      <t>キゴウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>エラーにならない～～！</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>（記／号）～</t>
+    <rPh sb="1" eb="2">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ゴウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>日本語！</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -407,9 +438,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
   <cols>
@@ -477,6 +510,27 @@
         <v>11</v>
       </c>
     </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
--array-split option extended to N dimensions
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\xlsx2json\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yhata\OneDrive\デスクトップ\GIT\xlsx2json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4735BC57-85B0-404E-8969-955C4FB26ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED00B59-CED3-4C15-93C2-0BA8C8493E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,21 +25,10 @@
     <definedName name="json.日本語_._記_号__">Sheet1!$G$11</definedName>
     <definedName name="json.日本語_.記号_">Sheet1!$G$10</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -67,10 +56,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>H3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>H5</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -119,11 +104,18 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>H2a,H2b</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>G3a,G3b</t>
+    <t>H2a1,H2b1
+H2a2,H2b2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>H3a1
+H3a2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>G3a1,G3b1
+G3a2</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -167,8 +159,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -452,94 +450,96 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="6" width="2.75" customWidth="1"/>
+    <col min="1" max="6" width="2.69921875" style="1" customWidth="1"/>
+    <col min="7" max="8" width="13.5" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="B2" t="s">
+    <row r="2" spans="1:8" ht="36">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="36">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="B3" t="s">
+    <row r="4" spans="1:8">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
+    </row>
+    <row r="5" spans="1:8">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" t="s">
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
+      <c r="G7" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="B8" t="s">
+      <c r="G8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G8" t="s">
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="B10" t="s">
+    <row r="11" spans="1:8">
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="G10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement --transform option and integrate --array-split option as “split:” conversion type
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,22 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yhata\OneDrive\デスクトップ\GIT\xlsx2json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED00B59-CED3-4C15-93C2-0BA8C8493E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17402E48-1009-4388-B6B5-FB83577A7763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="json.closed" localSheetId="1">Sheet2!$B$1</definedName>
     <definedName name="json.customer.address">Sheet1!$G$8</definedName>
     <definedName name="json.customer.name">Sheet1!$G$7</definedName>
+    <definedName name="json.opened">Sheet2!$B$2</definedName>
     <definedName name="json.parent.1">Sheet1!$G$2:$H$2</definedName>
     <definedName name="json.parent.2">Sheet1!$G$3:$H$3</definedName>
     <definedName name="json.parent.3">Sheet1!$G$4:$H$4</definedName>
     <definedName name="json.parent.4">Sheet1!$G$5:$H$5</definedName>
     <definedName name="json.日本語_._記_号__">Sheet1!$G$11</definedName>
     <definedName name="json.日本語_.記号_">Sheet1!$G$10</definedName>
+    <definedName name="otherprefix.test">Sheet1!$G$14</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>parent</t>
     <phoneticPr fontId="1"/>
@@ -104,19 +108,46 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>H2a1,H2b1
-H2a2,H2b2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>H3a1
 H3a2</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>G3a1,G3b1
+    <t>opened</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>closed</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>val_closed</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>val_opened</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>test</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>otherprefix:</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>otherprefix-test</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>H2a1, H2b1
+H2a2, H2b2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>G3a1, G3b1
 G3a2</t>
-    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -447,11 +478,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
   <cols>
@@ -473,7 +502,7 @@
         <v>3</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="36">
@@ -481,10 +510,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -540,6 +569,19 @@
       </c>
       <c r="G11" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -547,4 +589,36 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B65A99-14ED-4197-AB82-DC4CBE6267BB}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
support nested json, support datetime as iso8601
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yhata\OneDrive\デスクトップ\GIT\xlsx2json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198D8C37-91EB-4384-AA66-9D95B71BC7E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B2F365-C107-4BEB-A4DA-974F2CE25CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,19 +18,21 @@
   </sheets>
   <definedNames>
     <definedName name="json.closed" localSheetId="1">Sheet2!$B$1</definedName>
-    <definedName name="json.command_test">Sheet1!$J$15</definedName>
+    <definedName name="json.command_test">Sheet1!$J$16</definedName>
     <definedName name="json.customer.address">Sheet1!$J$8</definedName>
     <definedName name="json.customer.name">Sheet1!$J$7</definedName>
+    <definedName name="json.datetime">Sheet1!$J$14</definedName>
     <definedName name="json.num">Sheet1!$J$13</definedName>
     <definedName name="json.opened">Sheet2!$B$2</definedName>
     <definedName name="json.parent.1">Sheet1!$J$2:$K$2</definedName>
     <definedName name="json.parent.2">Sheet1!$J$3:$K$3</definedName>
     <definedName name="json.parent.3">Sheet1!$J$4:$K$4</definedName>
     <definedName name="json.parent.4">Sheet1!$J$5:$K$5</definedName>
-    <definedName name="json.v.e.r.y.v.e.r.y.d.e.e.p.p.a.t.h">Sheet1!$J$16</definedName>
+    <definedName name="json.time">Sheet1!$J$15</definedName>
+    <definedName name="json.v.e.r.y.v.e.r.y.d.e.e.p.p.a.t.h">Sheet1!$J$17</definedName>
     <definedName name="json.日本語_._記_号__">Sheet1!$J$11</definedName>
     <definedName name="json.日本語_.記号_">Sheet1!$J$10</definedName>
-    <definedName name="otherprefix.test">Sheet1!$J$19</definedName>
+    <definedName name="otherprefix.test">Sheet1!$J$20</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>parent</t>
     <phoneticPr fontId="1"/>
@@ -178,11 +180,18 @@
 テスト1</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>time</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="180" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -219,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -232,6 +241,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -513,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -625,32 +637,40 @@
         <v>45857</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="54">
+    <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" s="5">
+        <v>0.52425925925925931</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="54">
+      <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="J16" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:10">
+      <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Handle overlapping JSON paths by preserving values in __value__ key
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yhata\OneDrive\デスクトップ\GIT\xlsx2json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B2F365-C107-4BEB-A4DA-974F2CE25CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAA8ADB-88DD-4181-9929-71A757C4B2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,10 +29,12 @@
     <definedName name="json.parent.3">Sheet1!$J$4:$K$4</definedName>
     <definedName name="json.parent.4">Sheet1!$J$5:$K$5</definedName>
     <definedName name="json.time">Sheet1!$J$15</definedName>
+    <definedName name="json.v.e.r.y.v.e.r.y.d.e.e.p">Sheet1!$J$18</definedName>
     <definedName name="json.v.e.r.y.v.e.r.y.d.e.e.p.p.a.t.h">Sheet1!$J$17</definedName>
+    <definedName name="json.v.e.r.y.v.e.r.y.d.e.e.p.v1">Sheet1!$J$19</definedName>
     <definedName name="json.日本語_._記_号__">Sheet1!$J$11</definedName>
     <definedName name="json.日本語_.記号_">Sheet1!$J$10</definedName>
-    <definedName name="otherprefix.test">Sheet1!$J$20</definedName>
+    <definedName name="otherprefix.test">Sheet1!$J$22</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>parent</t>
     <phoneticPr fontId="1"/>
@@ -159,10 +161,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>deeppath-value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>num</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -182,6 +180,26 @@
   </si>
   <si>
     <t>time</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>veryverydeeppath-value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>veryverydeep-value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>v.e.r.y.v.e.r.y.d.e.e.p</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>v.e.r.y.v.e.r.y.d.e.e.p.v1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>veryverydeepv1-value</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -525,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -622,7 +640,7 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J13" s="1">
         <v>123</v>
@@ -630,7 +648,7 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J14" s="3">
         <f ca="1">TODAY()</f>
@@ -639,7 +657,7 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J15" s="5">
         <v>0.52425925925925931</v>
@@ -647,10 +665,10 @@
     </row>
     <row r="16" spans="1:11" ht="54">
       <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J16" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -658,19 +676,36 @@
         <v>24</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="17.399999999999999" customHeight="1"/>
+    <row r="21" spans="1:10">
+      <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="1" t="s">
+    <row r="22" spans="1:10">
+      <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>